<commit_message>
overview on all available strains of C. striatum #3
</commit_message>
<xml_diff>
--- a/data/strain_overview.xlsx
+++ b/data/strain_overview.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7C93CC6-3FB9-D945-9D10-C30CE6C8A989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E14068-E864-7E49-861A-BC7A65AB4C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2240" windowWidth="28040" windowHeight="17360" xr2:uid="{6BB749E6-D38B-CC4A-8935-4A8BC6B4CAF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>overview</t>
   </si>
@@ -149,6 +149,18 @@
   </si>
   <si>
     <t>Sequencing Year</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>Genes</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Size bp</t>
   </si>
 </sst>
 </file>
@@ -227,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -239,6 +251,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -554,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F487AC-71B5-624D-BBE3-662CD05273BB}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,7 +586,7 @@
     <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,8 +615,20 @@
       <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -634,8 +659,20 @@
       <c r="K2">
         <v>2021</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="11">
+        <v>2952500</v>
+      </c>
+      <c r="M2">
+        <v>59</v>
+      </c>
+      <c r="N2" s="11">
+        <v>2783</v>
+      </c>
+      <c r="O2" s="11">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -660,8 +697,20 @@
       <c r="K3">
         <v>2021</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="11">
+        <v>2948781</v>
+      </c>
+      <c r="M3">
+        <v>59</v>
+      </c>
+      <c r="N3" s="11">
+        <v>2830</v>
+      </c>
+      <c r="O3" s="11">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D4">
         <v>16</v>
       </c>
@@ -686,8 +735,20 @@
       <c r="K4">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="11">
+        <v>2904831</v>
+      </c>
+      <c r="M4">
+        <v>59</v>
+      </c>
+      <c r="N4" s="11">
+        <v>2716</v>
+      </c>
+      <c r="O4" s="11">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D5">
         <v>17</v>
       </c>
@@ -709,11 +770,23 @@
       <c r="K5">
         <v>2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="11">
+        <v>2665682</v>
+      </c>
+      <c r="M5">
+        <v>59</v>
+      </c>
+      <c r="N5" s="11">
+        <v>2471</v>
+      </c>
+      <c r="O5" s="11">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
@@ -733,11 +806,23 @@
       <c r="K7" s="5">
         <v>2017</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="11">
+        <v>2758500</v>
+      </c>
+      <c r="M7" s="7">
+        <v>59</v>
+      </c>
+      <c r="N7" s="11">
+        <v>2653</v>
+      </c>
+      <c r="O7" s="11">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
@@ -756,7 +841,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C10" s="8"/>
       <c r="E10" s="7">
         <v>216</v>
@@ -768,7 +853,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C11" s="8"/>
       <c r="E11" s="7" t="s">
         <v>25</v>
@@ -784,7 +869,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>33</v>
       </c>

</xml_diff>